<commit_message>
EBI - Mar TS
</commit_message>
<xml_diff>
--- a/SRA Documents/Manual Testing/Functional Testing/Stripe Fee logic.xlsx
+++ b/SRA Documents/Manual Testing/Functional Testing/Stripe Fee logic.xlsx
@@ -424,7 +424,7 @@
   <dimension ref="C2:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -453,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>50.5</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>3</v>
@@ -482,7 +482,7 @@
       </c>
       <c r="G6">
         <f xml:space="preserve"> D3 * (G3- J3) - (M3)</f>
-        <v>1.7000000000000004</v>
+        <v>0.71000000000000019</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>6</v>
@@ -497,7 +497,7 @@
       </c>
       <c r="G8">
         <f>D3*(J3)+(M3)</f>
-        <v>3.1999999999999997</v>
+        <v>1.7645</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>6</v>
@@ -512,7 +512,7 @@
       </c>
       <c r="G10">
         <f>G6+G8</f>
-        <v>4.9000000000000004</v>
+        <v>2.4744999999999999</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>6</v>

</xml_diff>